<commit_message>
Fixed edge case involving date time string with seconds.
When supplying a date time string with seconds (11/5/2013 11:45:00), the resulting DateTime object would not round the fractional seconds resulting in a time string of 11/5/2013 11:44:59. 

Time is now properly rounded before returning the DateTime object.
</commit_message>
<xml_diff>
--- a/test/files/datetime.xlsx
+++ b/test/files/datetime.xlsx
@@ -1,29 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="233"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="233"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy\ h:mm:ss;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -45,16 +65,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,18 +435,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -480,6 +507,17 @@
       </c>
       <c r="C7" s="1">
         <v>22606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>41583.489583333299</v>
+      </c>
+      <c r="B8" s="3">
+        <v>41583.489583333299</v>
+      </c>
+      <c r="C8" s="3">
+        <v>41583.489583333299</v>
       </c>
     </row>
   </sheetData>
@@ -489,16 +527,21 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -506,16 +549,21 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -523,5 +571,10 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>